<commit_message>
create: new irregular contract features
</commit_message>
<xml_diff>
--- a/Work/data/irregular_contracts/whitelist.xlsx
+++ b/Work/data/irregular_contracts/whitelist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levin/workspace/git-repositories/anaconda/study-pandas-tutorials/Work/data/irregular_contracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84938332-0B52-CA47-B637-3F2D3E4A4898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DA6433-FC94-4640-8DF1-AE1DE2E7AA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1500" windowWidth="27440" windowHeight="15520" xr2:uid="{2586D083-F5E0-D74A-96FE-0BAAF84BB202}"/>
   </bookViews>
@@ -37,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>合同编号</t>
-  </si>
-  <si>
     <t>qsnhdzx-2022-02-0066</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>科技园YX-Z-[2022]006</t>
+  </si>
+  <si>
+    <t>contract_no</t>
   </si>
 </sst>
 </file>
@@ -460,9 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4FE57B-0F32-7C47-9790-5A6552A22B77}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -471,47 +469,47 @@
   <sheetData>
     <row r="1" spans="1:1" ht="17">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="17">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="17">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="17">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="17">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="17">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="17">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>